<commit_message>
Update to perk database
</commit_message>
<xml_diff>
--- a/Perk_data/data/classic/classic_healing_perks.xlsx
+++ b/Perk_data/data/classic/classic_healing_perks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre-Luc\Documents\GitHub\BattleBay_tool\Perk_data\data\classic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94E994B-36A9-472D-8F8E-15F800805A9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8487BBAC-1853-415B-AA1E-2ACB31147C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17ED7760-9FD3-4054-A926-911402D2CD26}"/>
   </bookViews>
@@ -98,7 +98,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +126,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -191,10 +197,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,7 +714,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,68 +736,68 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
maj perk data use
</commit_message>
<xml_diff>
--- a/Perk_data/data/classic/classic_healing_perks.xlsx
+++ b/Perk_data/data/classic/classic_healing_perks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pierre-Luc\Documents\GitHub\BattleBay_tool\Perk_data\data\classic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8487BBAC-1853-415B-AA1E-2ACB31147C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF145B73-3F20-4B6B-AB71-D7ADB87A8144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17ED7760-9FD3-4054-A926-911402D2CD26}"/>
   </bookViews>
@@ -48,15 +48,6 @@
     <t>1st-Bonus</t>
   </si>
   <si>
-    <t>Epic</t>
-  </si>
-  <si>
-    <t>Rare</t>
-  </si>
-  <si>
-    <t>Uncommon</t>
-  </si>
-  <si>
     <t>7.50%-BASE_STAT</t>
   </si>
   <si>
@@ -76,6 +67,15 @@
   </si>
   <si>
     <t>all_repair_item</t>
+  </si>
+  <si>
+    <t>epic</t>
+  </si>
+  <si>
+    <t>rare</t>
+  </si>
+  <si>
+    <t>uncommon</t>
   </si>
 </sst>
 </file>
@@ -221,197 +221,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>5715</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>325755</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2900DEF2-74E0-421C-9275-6E34F9A1B0D8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5293995" y="190500"/>
-          <a:ext cx="3368040" cy="3962401"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="2400" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>READ FIRST</a:t>
-          </a:r>
-          <a:endParaRPr lang="fr-FR" sz="2400">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>The goal of this drive and excel is to have an up to date list of all the perks in all possible rarities. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>Here the legendaries have the right values and thus are colored in light green.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>The goal is for you to go around your stuff and check if your perks are already updated. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>If they are not updated here, they will not be colored (in the excel) and then you have the oportunity to either dm me on discord with a screeshot of the perk's infos so I change it my self (@komiko44240 on the official battle bay discord sever), or change it yourself (if I can figure out a way to let google drive alow you to do that)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>And please if you change any value that was not modified already, color it with the right (or as close as possible) color (R: 226 G:239 B:218 or hex</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>: #e2efda</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>). </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>If  the perk that you have is not part of this list, please dm me directly on discord (@komiko44240 on the official battle bay discord sever) without modifying</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t> any thing here.</a:t>
-          </a:r>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100"/>
-            <a:t>Note : If</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
-            <a:t> any modification apported to this spread sheet is childish you will be banned from accesing this drive</a:t>
-          </a:r>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -714,7 +523,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,73 +546,72 @@
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C13" xr:uid="{043BCFDB-ACF3-4DBE-A0C0-8C4B7FE8841E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>